<commit_message>
update to get_assignments and definition
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/Projects/virtual_assistant/Best_Senior_Project/FSCVA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\FSCVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3A478-3F67-AE4E-9494-0D6B64408AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7177A14-F252-4355-9245-4E16DED2500C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="8760" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="167">
   <si>
     <t>get_weather</t>
   </si>
@@ -524,6 +524,18 @@
   </si>
   <si>
     <t>broken</t>
+  </si>
+  <si>
+    <t>google_search</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>google search</t>
+  </si>
+  <si>
+    <t>search on google</t>
   </si>
 </sst>
 </file>
@@ -878,28 +890,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,8 +951,11 @@
       <c r="M1" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -980,8 +995,11 @@
       <c r="M2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1021,8 +1039,11 @@
       <c r="M3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1062,8 +1083,11 @@
       <c r="M4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1104,7 +1128,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1169,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1183,7 +1207,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +1239,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1268,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1270,7 +1294,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1290,7 +1314,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1307,7 +1331,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1324,7 +1348,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1341,7 +1365,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1355,7 +1379,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1383,7 +1407,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1397,7 +1421,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1411,7 +1435,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>77</v>
       </c>
@@ -1419,7 +1443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>74</v>
       </c>
@@ -1427,7 +1451,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>76</v>
       </c>
@@ -1435,7 +1459,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>75</v>
       </c>
@@ -1443,22 +1467,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
tweaked confidence for google_search for better accuracy
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\FSCVA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/Projects/virtual_assistant/Best_Senior_Project/FSCVA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7177A14-F252-4355-9245-4E16DED2500C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B5C49C-6D22-3B4B-9CFF-2F776D497393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
   <si>
     <t>get_weather</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>search on google</t>
+  </si>
+  <si>
+    <t>bing</t>
   </si>
 </sst>
 </file>
@@ -892,26 +895,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +960,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -999,7 +1004,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1043,7 +1048,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1087,7 +1092,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1127,8 +1132,11 @@
       <c r="M5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1168,8 +1176,11 @@
       <c r="M6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1206,8 +1217,11 @@
       <c r="M7" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1238,8 +1252,11 @@
       <c r="M8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1267,8 +1284,11 @@
       <c r="M9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1293,8 +1313,11 @@
       <c r="M10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1313,8 +1336,11 @@
       <c r="M11" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1330,8 +1356,11 @@
       <c r="L12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1347,8 +1376,11 @@
       <c r="L13" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1365,7 +1397,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1411,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1425,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1407,7 +1439,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1421,7 +1453,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1435,7 +1467,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>77</v>
       </c>
@@ -1443,7 +1475,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>74</v>
       </c>
@@ -1451,7 +1483,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>76</v>
       </c>
@@ -1459,7 +1491,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>75</v>
       </c>
@@ -1467,22 +1499,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
merge changes with current main
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\FSCVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7177A14-F252-4355-9245-4E16DED2500C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D378B8-B0F9-4A2D-B89E-35C9C0445B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="168">
   <si>
     <t>get_weather</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>search on google</t>
+  </si>
+  <si>
+    <t>lookup</t>
   </si>
 </sst>
 </file>
@@ -892,26 +895,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +958,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1043,7 +1046,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1127,8 +1130,11 @@
       <c r="M5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1331,7 +1337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1407,7 +1413,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>77</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>74</v>
       </c>
@@ -1451,7 +1457,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>76</v>
       </c>
@@ -1459,7 +1465,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>75</v>
       </c>
@@ -1467,22 +1473,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
fixed issue with get_balance
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/Projects/virtual_assistant/Best_Senior_Project/FSCVA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5928120D-6D0D-694C-BEFA-1DEE8C37E19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD26C42D-5CB5-4A4C-89B8-DB4BA43C2E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="174">
   <si>
     <t>get_weather</t>
   </si>
@@ -551,6 +551,12 @@
   </si>
   <si>
     <t>wake_up</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>point</t>
   </si>
 </sst>
 </file>
@@ -907,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,6 +1520,9 @@
       <c r="D20" t="s">
         <v>77</v>
       </c>
+      <c r="E20" t="s">
+        <v>172</v>
+      </c>
       <c r="L20" t="s">
         <v>155</v>
       </c>
@@ -1522,6 +1531,9 @@
       <c r="D21" t="s">
         <v>74</v>
       </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
       <c r="L21" t="s">
         <v>156</v>
       </c>
@@ -1529,6 +1541,9 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>173</v>
       </c>
       <c r="L22" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
almost project ready, all warnings gone and google working
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/Projects/virtual_assistant/Best_Senior_Project/FSCVA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\FSCVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD26C42D-5CB5-4A4C-89B8-DB4BA43C2E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A010049-C1A3-4DAE-B172-3F0AC2E1D213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -913,29 +913,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +982,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>77</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>74</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>76</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>75</v>
       </c>
@@ -1557,22 +1557,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
filled out testing database
</commit_message>
<xml_diff>
--- a/FSCVA/intents.xlsx
+++ b/FSCVA/intents.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\FSCVA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklausauen/Desktop/School - 16th/Senior Project/virtual_assistant/Best_Senior_Project/FSCVA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A010049-C1A3-4DAE-B172-3F0AC2E1D213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06295A1D-2BC6-0244-BBC7-9230830C2BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -913,29 +914,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +983,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1409,7 +1410,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>77</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>74</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>76</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>75</v>
       </c>
@@ -1557,22 +1558,22 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>134</v>
       </c>

</xml_diff>